<commit_message>
logic ok. jitters modified. timing test needed
</commit_message>
<xml_diff>
--- a/StimuliTable-Recognition_4-blocks_48-pairs_cont-loc_12345-delays.xlsx
+++ b/StimuliTable-Recognition_4-blocks_48-pairs_cont-loc_12345-delays.xlsx
@@ -268,17 +268,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -382,8 +372,8 @@
   </sheetPr>
   <dimension ref="A1:Z145"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A104" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L110" activeCellId="0" sqref="L110:L145"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A115" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -391,7 +381,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.7"/>
@@ -404,11 +394,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="23.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="0" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="21" style="0" width="23.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="21" style="0" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="23.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="29.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="32.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="35.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="35.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="32" style="0" width="8.67"/>
   </cols>
   <sheetData>
@@ -500,7 +490,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1</v>
@@ -523,7 +513,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1</v>
@@ -546,7 +536,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>1</v>
@@ -569,7 +559,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1</v>
@@ -592,7 +582,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>1000</v>
+        <v>5000</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>1</v>
@@ -615,7 +605,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>3000</v>
+        <v>8000</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>1</v>
@@ -661,7 +651,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>1</v>
@@ -684,7 +674,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>1</v>
@@ -707,7 +697,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>1</v>
@@ -730,7 +720,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>1000</v>
+        <v>4000</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>1</v>
@@ -776,7 +766,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>1</v>
@@ -822,7 +812,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>1</v>
@@ -845,7 +835,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>1</v>
@@ -868,7 +858,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>1000</v>
+        <v>4000</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>1</v>
@@ -891,7 +881,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>1</v>
@@ -914,7 +904,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>1</v>
@@ -937,7 +927,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>1</v>
@@ -983,7 +973,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>6000</v>
+        <v>1000</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>1</v>
@@ -1029,7 +1019,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>1</v>
@@ -1121,7 +1111,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>1</v>
@@ -1144,7 +1134,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>1</v>
@@ -1190,7 +1180,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>1</v>
@@ -1213,7 +1203,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>1</v>
@@ -1236,7 +1226,7 @@
         <v>33</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>1</v>
@@ -1259,7 +1249,7 @@
         <v>34</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>1</v>
@@ -1305,7 +1295,7 @@
         <v>36</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>1</v>
@@ -1328,7 +1318,7 @@
         <v>37</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>500</v>
+        <v>3000</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>2</v>
@@ -1351,7 +1341,7 @@
         <v>38</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="E39" s="0" t="n">
         <v>2</v>
@@ -1374,7 +1364,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>2</v>
@@ -1420,7 +1410,7 @@
         <v>41</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="E42" s="0" t="n">
         <v>2</v>
@@ -1443,7 +1433,7 @@
         <v>42</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E43" s="0" t="n">
         <v>2</v>
@@ -1466,7 +1456,7 @@
         <v>43</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>2</v>
@@ -1512,7 +1502,7 @@
         <v>45</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>2</v>
@@ -1535,7 +1525,7 @@
         <v>46</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="E47" s="0" t="n">
         <v>2</v>
@@ -1558,7 +1548,7 @@
         <v>47</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="E48" s="0" t="n">
         <v>2</v>
@@ -1581,7 +1571,7 @@
         <v>48</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="E49" s="0" t="n">
         <v>2</v>
@@ -1604,7 +1594,7 @@
         <v>49</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>2</v>
@@ -1627,7 +1617,7 @@
         <v>50</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="E51" s="0" t="n">
         <v>2</v>
@@ -1650,7 +1640,7 @@
         <v>51</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="E52" s="0" t="n">
         <v>2</v>
@@ -1673,7 +1663,7 @@
         <v>52</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="E53" s="0" t="n">
         <v>2</v>
@@ -1696,7 +1686,7 @@
         <v>53</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="E54" s="0" t="n">
         <v>2</v>
@@ -1719,7 +1709,7 @@
         <v>54</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>6000</v>
+        <v>1000</v>
       </c>
       <c r="E55" s="0" t="n">
         <v>2</v>
@@ -1742,7 +1732,7 @@
         <v>55</v>
       </c>
       <c r="C56" s="0" t="n">
-        <v>500</v>
+        <v>3000</v>
       </c>
       <c r="E56" s="0" t="n">
         <v>2</v>
@@ -1765,7 +1755,7 @@
         <v>56</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="E57" s="0" t="n">
         <v>2</v>
@@ -1811,7 +1801,7 @@
         <v>58</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E59" s="0" t="n">
         <v>2</v>
@@ -1834,7 +1824,7 @@
         <v>59</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="E60" s="0" t="n">
         <v>2</v>
@@ -1857,7 +1847,7 @@
         <v>60</v>
       </c>
       <c r="C61" s="0" t="n">
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="E61" s="0" t="n">
         <v>2</v>
@@ -1880,7 +1870,7 @@
         <v>61</v>
       </c>
       <c r="C62" s="0" t="n">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="E62" s="0" t="n">
         <v>2</v>
@@ -1903,7 +1893,7 @@
         <v>62</v>
       </c>
       <c r="C63" s="0" t="n">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="E63" s="0" t="n">
         <v>2</v>
@@ -1926,7 +1916,7 @@
         <v>63</v>
       </c>
       <c r="C64" s="0" t="n">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="E64" s="0" t="n">
         <v>2</v>
@@ -1949,7 +1939,7 @@
         <v>64</v>
       </c>
       <c r="C65" s="0" t="n">
-        <v>2000</v>
+        <v>8000</v>
       </c>
       <c r="E65" s="0" t="n">
         <v>2</v>
@@ -1972,7 +1962,7 @@
         <v>65</v>
       </c>
       <c r="C66" s="0" t="n">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="E66" s="0" t="n">
         <v>2</v>
@@ -1995,7 +1985,7 @@
         <v>66</v>
       </c>
       <c r="C67" s="0" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="E67" s="0" t="n">
         <v>2</v>
@@ -2041,7 +2031,7 @@
         <v>68</v>
       </c>
       <c r="C69" s="0" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="E69" s="0" t="n">
         <v>2</v>
@@ -2064,7 +2054,7 @@
         <v>69</v>
       </c>
       <c r="C70" s="0" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E70" s="0" t="n">
         <v>2</v>
@@ -2087,7 +2077,7 @@
         <v>70</v>
       </c>
       <c r="C71" s="0" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E71" s="0" t="n">
         <v>2</v>
@@ -2110,7 +2100,7 @@
         <v>71</v>
       </c>
       <c r="C72" s="0" t="n">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="E72" s="0" t="n">
         <v>2</v>
@@ -2156,7 +2146,7 @@
         <v>73</v>
       </c>
       <c r="C74" s="0" t="n">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="E74" s="0" t="n">
         <v>3</v>
@@ -2183,7 +2173,7 @@
         <v>74</v>
       </c>
       <c r="C75" s="0" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E75" s="0" t="n">
         <v>3</v>
@@ -2237,7 +2227,7 @@
         <v>76</v>
       </c>
       <c r="C77" s="0" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E77" s="0" t="n">
         <v>3</v>
@@ -2264,7 +2254,7 @@
         <v>77</v>
       </c>
       <c r="C78" s="0" t="n">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="E78" s="0" t="n">
         <v>3</v>
@@ -2291,7 +2281,7 @@
         <v>78</v>
       </c>
       <c r="C79" s="0" t="n">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="E79" s="0" t="n">
         <v>3</v>
@@ -2318,7 +2308,7 @@
         <v>79</v>
       </c>
       <c r="C80" s="0" t="n">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="E80" s="0" t="n">
         <v>3</v>
@@ -2345,7 +2335,7 @@
         <v>80</v>
       </c>
       <c r="C81" s="0" t="n">
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="E81" s="0" t="n">
         <v>3</v>
@@ -2453,7 +2443,7 @@
         <v>84</v>
       </c>
       <c r="C85" s="0" t="n">
-        <v>1000</v>
+        <v>8000</v>
       </c>
       <c r="E85" s="0" t="n">
         <v>3</v>
@@ -2507,7 +2497,7 @@
         <v>86</v>
       </c>
       <c r="C87" s="0" t="n">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="E87" s="0" t="n">
         <v>3</v>
@@ -2561,7 +2551,7 @@
         <v>88</v>
       </c>
       <c r="C89" s="0" t="n">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="E89" s="0" t="n">
         <v>3</v>
@@ -2642,7 +2632,7 @@
         <v>91</v>
       </c>
       <c r="C92" s="0" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="E92" s="0" t="n">
         <v>3</v>
@@ -2696,7 +2686,7 @@
         <v>93</v>
       </c>
       <c r="C94" s="0" t="n">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="E94" s="0" t="n">
         <v>3</v>
@@ -2723,7 +2713,7 @@
         <v>94</v>
       </c>
       <c r="C95" s="0" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E95" s="0" t="n">
         <v>3</v>
@@ -2750,7 +2740,7 @@
         <v>95</v>
       </c>
       <c r="C96" s="0" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E96" s="0" t="n">
         <v>3</v>
@@ -2777,7 +2767,7 @@
         <v>96</v>
       </c>
       <c r="C97" s="0" t="n">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="E97" s="0" t="n">
         <v>3</v>
@@ -2804,7 +2794,7 @@
         <v>97</v>
       </c>
       <c r="C98" s="0" t="n">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="E98" s="0" t="n">
         <v>3</v>
@@ -2831,7 +2821,7 @@
         <v>98</v>
       </c>
       <c r="C99" s="0" t="n">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="E99" s="0" t="n">
         <v>3</v>
@@ -2858,7 +2848,7 @@
         <v>99</v>
       </c>
       <c r="C100" s="0" t="n">
-        <v>3000</v>
+        <v>500</v>
       </c>
       <c r="E100" s="0" t="n">
         <v>3</v>
@@ -2912,7 +2902,7 @@
         <v>101</v>
       </c>
       <c r="C102" s="0" t="n">
-        <v>1000</v>
+        <v>4000</v>
       </c>
       <c r="E102" s="0" t="n">
         <v>3</v>
@@ -2939,7 +2929,7 @@
         <v>102</v>
       </c>
       <c r="C103" s="0" t="n">
-        <v>6000</v>
+        <v>3000</v>
       </c>
       <c r="E103" s="0" t="n">
         <v>3</v>
@@ -2966,7 +2956,7 @@
         <v>103</v>
       </c>
       <c r="C104" s="0" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E104" s="0" t="n">
         <v>3</v>
@@ -2993,7 +2983,7 @@
         <v>104</v>
       </c>
       <c r="C105" s="0" t="n">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="E105" s="0" t="n">
         <v>3</v>
@@ -3020,7 +3010,7 @@
         <v>105</v>
       </c>
       <c r="C106" s="0" t="n">
-        <v>1000</v>
+        <v>4000</v>
       </c>
       <c r="E106" s="0" t="n">
         <v>3</v>
@@ -3047,7 +3037,7 @@
         <v>106</v>
       </c>
       <c r="C107" s="0" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E107" s="0" t="n">
         <v>3</v>
@@ -3101,7 +3091,7 @@
         <v>108</v>
       </c>
       <c r="C109" s="0" t="n">
-        <v>1000</v>
+        <v>4000</v>
       </c>
       <c r="E109" s="0" t="n">
         <v>3</v>
@@ -3128,7 +3118,7 @@
         <v>109</v>
       </c>
       <c r="C110" s="0" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E110" s="0" t="n">
         <v>4</v>
@@ -3174,7 +3164,7 @@
         <v>111</v>
       </c>
       <c r="C112" s="0" t="n">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="E112" s="0" t="n">
         <v>4</v>
@@ -3197,7 +3187,7 @@
         <v>112</v>
       </c>
       <c r="C113" s="0" t="n">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="E113" s="0" t="n">
         <v>4</v>
@@ -3220,7 +3210,7 @@
         <v>113</v>
       </c>
       <c r="C114" s="0" t="n">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="E114" s="0" t="n">
         <v>4</v>
@@ -3243,7 +3233,7 @@
         <v>114</v>
       </c>
       <c r="C115" s="0" t="n">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="E115" s="0" t="n">
         <v>4</v>
@@ -3266,7 +3256,7 @@
         <v>115</v>
       </c>
       <c r="C116" s="0" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="E116" s="0" t="n">
         <v>4</v>
@@ -3312,7 +3302,7 @@
         <v>117</v>
       </c>
       <c r="C118" s="0" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E118" s="0" t="n">
         <v>4</v>
@@ -3335,7 +3325,7 @@
         <v>118</v>
       </c>
       <c r="C119" s="0" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="E119" s="0" t="n">
         <v>4</v>
@@ -3358,7 +3348,7 @@
         <v>119</v>
       </c>
       <c r="C120" s="0" t="n">
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="E120" s="0" t="n">
         <v>4</v>
@@ -3381,7 +3371,7 @@
         <v>120</v>
       </c>
       <c r="C121" s="0" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="E121" s="0" t="n">
         <v>4</v>
@@ -3427,7 +3417,7 @@
         <v>122</v>
       </c>
       <c r="C123" s="0" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E123" s="0" t="n">
         <v>4</v>
@@ -3450,7 +3440,7 @@
         <v>123</v>
       </c>
       <c r="C124" s="0" t="n">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="E124" s="0" t="n">
         <v>4</v>
@@ -3519,7 +3509,7 @@
         <v>126</v>
       </c>
       <c r="C127" s="0" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="E127" s="0" t="n">
         <v>4</v>
@@ -3542,7 +3532,7 @@
         <v>127</v>
       </c>
       <c r="C128" s="0" t="n">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="E128" s="0" t="n">
         <v>4</v>
@@ -3565,7 +3555,7 @@
         <v>128</v>
       </c>
       <c r="C129" s="0" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E129" s="0" t="n">
         <v>4</v>
@@ -3588,7 +3578,7 @@
         <v>129</v>
       </c>
       <c r="C130" s="0" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="E130" s="0" t="n">
         <v>4</v>
@@ -3611,7 +3601,7 @@
         <v>130</v>
       </c>
       <c r="C131" s="0" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E131" s="0" t="n">
         <v>4</v>
@@ -3634,7 +3624,7 @@
         <v>131</v>
       </c>
       <c r="C132" s="0" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E132" s="0" t="n">
         <v>4</v>
@@ -3657,7 +3647,7 @@
         <v>132</v>
       </c>
       <c r="C133" s="0" t="n">
-        <v>6000</v>
+        <v>1000</v>
       </c>
       <c r="E133" s="0" t="n">
         <v>4</v>
@@ -3680,7 +3670,7 @@
         <v>133</v>
       </c>
       <c r="C134" s="0" t="n">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="E134" s="0" t="n">
         <v>4</v>
@@ -3703,7 +3693,7 @@
         <v>134</v>
       </c>
       <c r="C135" s="0" t="n">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="E135" s="0" t="n">
         <v>4</v>
@@ -3726,7 +3716,7 @@
         <v>135</v>
       </c>
       <c r="C136" s="0" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E136" s="0" t="n">
         <v>4</v>
@@ -3749,7 +3739,7 @@
         <v>136</v>
       </c>
       <c r="C137" s="0" t="n">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="E137" s="0" t="n">
         <v>4</v>
@@ -3772,7 +3762,7 @@
         <v>137</v>
       </c>
       <c r="C138" s="0" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E138" s="0" t="n">
         <v>4</v>
@@ -3795,7 +3785,7 @@
         <v>138</v>
       </c>
       <c r="C139" s="0" t="n">
-        <v>3000</v>
+        <v>8000</v>
       </c>
       <c r="E139" s="0" t="n">
         <v>4</v>
@@ -3818,7 +3808,7 @@
         <v>139</v>
       </c>
       <c r="C140" s="0" t="n">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="E140" s="0" t="n">
         <v>4</v>
@@ -3841,7 +3831,7 @@
         <v>140</v>
       </c>
       <c r="C141" s="0" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E141" s="0" t="n">
         <v>4</v>
@@ -3887,7 +3877,7 @@
         <v>142</v>
       </c>
       <c r="C143" s="0" t="n">
-        <v>1000</v>
+        <v>6000</v>
       </c>
       <c r="E143" s="0" t="n">
         <v>4</v>
@@ -3910,7 +3900,7 @@
         <v>143</v>
       </c>
       <c r="C144" s="0" t="n">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="E144" s="0" t="n">
         <v>4</v>
@@ -3933,7 +3923,7 @@
         <v>144</v>
       </c>
       <c r="C145" s="0" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E145" s="0" t="n">
         <v>4</v>
@@ -3974,7 +3964,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="1" sqref="L110:L145 B14"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="1" sqref="C2:C145 B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4014,7 +4004,7 @@
       </c>
       <c r="E2" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.977958546245055</v>
+        <v>0.946311985684312</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4032,7 +4022,7 @@
       </c>
       <c r="E3" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.393108242279958</v>
+        <v>0.720209500680727</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4050,7 +4040,7 @@
       </c>
       <c r="E4" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.74046912698783</v>
+        <v>0.1481796082024</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4068,7 +4058,7 @@
       </c>
       <c r="E5" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.358794017221298</v>
+        <v>0.27083396816056</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4086,7 +4076,7 @@
       </c>
       <c r="E6" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.995023299363093</v>
+        <v>0.145360789050625</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4104,7 +4094,7 @@
       </c>
       <c r="E7" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.00503768549306084</v>
+        <v>0.0361140271331159</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4122,7 +4112,7 @@
       </c>
       <c r="E8" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.271195836149544</v>
+        <v>0.778833127346451</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4140,7 +4130,7 @@
       </c>
       <c r="E9" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.349466973951066</v>
+        <v>0.204433395294668</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4158,7 +4148,7 @@
       </c>
       <c r="E10" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.167678970166162</v>
+        <v>0.286039760399081</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4176,7 +4166,7 @@
       </c>
       <c r="E11" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.175400555104605</v>
+        <v>0.278948545411663</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4194,7 +4184,7 @@
       </c>
       <c r="E12" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.300343901265246</v>
+        <v>0.336280095736792</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4212,7 +4202,7 @@
       </c>
       <c r="E13" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.426681318379075</v>
+        <v>0.537077320658328</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4230,7 +4220,7 @@
       </c>
       <c r="E14" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.00476600930799622</v>
+        <v>0.096606009248852</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4248,7 +4238,7 @@
       </c>
       <c r="E15" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.713586986759681</v>
+        <v>0.512231414189414</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4266,7 +4256,7 @@
       </c>
       <c r="E16" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.147911847950174</v>
+        <v>0.123808179495145</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4284,7 +4274,7 @@
       </c>
       <c r="E17" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.705103978071637</v>
+        <v>0.757686416848898</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4302,7 +4292,7 @@
       </c>
       <c r="E18" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.795578822755222</v>
+        <v>0.744463759734675</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4320,7 +4310,7 @@
       </c>
       <c r="E19" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.10222340990778</v>
+        <v>0.244750258295131</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4338,7 +4328,7 @@
       </c>
       <c r="E20" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.203374359067175</v>
+        <v>0.948432434788298</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4356,7 +4346,7 @@
       </c>
       <c r="E21" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.410185261775822</v>
+        <v>0.410802138900173</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4374,7 +4364,7 @@
       </c>
       <c r="E22" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.100514066592862</v>
+        <v>0.298764080771577</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4392,7 +4382,7 @@
       </c>
       <c r="E23" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.768260394130679</v>
+        <v>0.00541902688963443</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4410,7 +4400,7 @@
       </c>
       <c r="E24" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.294427457547106</v>
+        <v>0.215297933397407</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4428,7 +4418,7 @@
       </c>
       <c r="E25" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.050199491427047</v>
+        <v>0.0894662812622269</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4446,7 +4436,7 @@
       </c>
       <c r="E26" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.318593677994541</v>
+        <v>0.983337072777042</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4464,7 +4454,7 @@
       </c>
       <c r="E27" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.679452349579383</v>
+        <v>0.780704407818466</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4482,7 +4472,7 @@
       </c>
       <c r="E28" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.959086614272027</v>
+        <v>0.809340798062265</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4500,7 +4490,7 @@
       </c>
       <c r="E29" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.968249311514551</v>
+        <v>0.610857099945572</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4518,7 +4508,7 @@
       </c>
       <c r="E30" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.00497986407026341</v>
+        <v>0.334674294593967</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4536,7 +4526,7 @@
       </c>
       <c r="E31" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.866598343090976</v>
+        <v>0.402399206644797</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4554,7 +4544,7 @@
       </c>
       <c r="E32" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.709038023211482</v>
+        <v>0.51949700798294</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4572,7 +4562,7 @@
       </c>
       <c r="E33" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.190361292756133</v>
+        <v>0.357223481335347</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4590,7 +4580,7 @@
       </c>
       <c r="E34" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.779622224740199</v>
+        <v>0.40471921260105</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4608,7 +4598,7 @@
       </c>
       <c r="E35" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.023737344756462</v>
+        <v>0.84777368650953</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4626,7 +4616,7 @@
       </c>
       <c r="E36" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.382694924598417</v>
+        <v>0.256377373152753</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4644,7 +4634,7 @@
       </c>
       <c r="E37" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.341889230295956</v>
+        <v>0.974482615290354</v>
       </c>
     </row>
   </sheetData>
@@ -4673,7 +4663,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="L110:L145 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4713,7 +4703,7 @@
       </c>
       <c r="E2" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.680182904929564</v>
+        <v>0.617510717757557</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4731,7 +4721,7 @@
       </c>
       <c r="E3" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.757810455568259</v>
+        <v>0.76088310364495</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4749,7 +4739,7 @@
       </c>
       <c r="E4" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0290209934513696</v>
+        <v>0.722016079256622</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4767,7 +4757,7 @@
       </c>
       <c r="E5" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.409206031639933</v>
+        <v>0.900089442732585</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4785,7 +4775,7 @@
       </c>
       <c r="E6" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.270709768583227</v>
+        <v>0.641305919118632</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4803,7 +4793,7 @@
       </c>
       <c r="E7" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.887860541720324</v>
+        <v>0.19762708995372</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4821,7 +4811,7 @@
       </c>
       <c r="E8" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.932053386863922</v>
+        <v>0.49756792241699</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4839,7 +4829,7 @@
       </c>
       <c r="E9" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.110968779961107</v>
+        <v>0.68584118616925</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4857,7 +4847,7 @@
       </c>
       <c r="E10" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.373094734101526</v>
+        <v>0.472150078611521</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4875,7 +4865,7 @@
       </c>
       <c r="E11" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.186048643807104</v>
+        <v>0.549306500727323</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4893,7 +4883,7 @@
       </c>
       <c r="E12" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.653666567598863</v>
+        <v>0.367228472614176</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4911,7 +4901,7 @@
       </c>
       <c r="E13" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.00783024320403133</v>
+        <v>0.687562336024388</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4929,7 +4919,7 @@
       </c>
       <c r="E14" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.522149546568267</v>
+        <v>0.152012013892299</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4947,7 +4937,7 @@
       </c>
       <c r="E15" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.540069597055089</v>
+        <v>0.798309076489667</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4965,7 +4955,7 @@
       </c>
       <c r="E16" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.928066140079433</v>
+        <v>0.378207013742374</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4983,7 +4973,7 @@
       </c>
       <c r="E17" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.837994231425628</v>
+        <v>0.00797531696009247</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5001,7 +4991,7 @@
       </c>
       <c r="E18" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.312088120145046</v>
+        <v>0.797421679376233</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5019,7 +5009,7 @@
       </c>
       <c r="E19" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.217888775726547</v>
+        <v>0.214611827399179</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5037,7 +5027,7 @@
       </c>
       <c r="E20" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0776529554338736</v>
+        <v>0.764010600562115</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5055,7 +5045,7 @@
       </c>
       <c r="E21" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.711510827664373</v>
+        <v>0.287734750339493</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5073,7 +5063,7 @@
       </c>
       <c r="E22" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0410309444200792</v>
+        <v>0.215482649382797</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5091,7 +5081,7 @@
       </c>
       <c r="E23" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.242447612708741</v>
+        <v>0.73255156562331</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5109,7 +5099,7 @@
       </c>
       <c r="E24" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.78513459373039</v>
+        <v>0.0815521304993709</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5127,7 +5117,7 @@
       </c>
       <c r="E25" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.763322479043025</v>
+        <v>0.562901076041282</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5145,7 +5135,7 @@
       </c>
       <c r="E26" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.444471889270827</v>
+        <v>0.674355991291607</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5163,7 +5153,7 @@
       </c>
       <c r="E27" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.422496507099404</v>
+        <v>0.149887005077455</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5181,7 +5171,7 @@
       </c>
       <c r="E28" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.651202368300778</v>
+        <v>0.373094163310402</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5199,7 +5189,7 @@
       </c>
       <c r="E29" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0349861312393512</v>
+        <v>0.497826583191261</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5217,7 +5207,7 @@
       </c>
       <c r="E30" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.867029619999484</v>
+        <v>0.570167489719721</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5235,7 +5225,7 @@
       </c>
       <c r="E31" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.558644402708707</v>
+        <v>0.524245763186294</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5253,7 +5243,7 @@
       </c>
       <c r="E32" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.70368562112046</v>
+        <v>0.724915732135317</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5271,7 +5261,7 @@
       </c>
       <c r="E33" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0532943227613478</v>
+        <v>0.907592333820743</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5289,7 +5279,7 @@
       </c>
       <c r="E34" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.690297307438173</v>
+        <v>0.404893252018201</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5307,7 +5297,7 @@
       </c>
       <c r="E35" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.714886504511341</v>
+        <v>0.462321489625543</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5325,7 +5315,7 @@
       </c>
       <c r="E36" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0806076185179297</v>
+        <v>0.311079640829937</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5343,7 +5333,7 @@
       </c>
       <c r="E37" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.694023059776782</v>
+        <v>0.203767024766847</v>
       </c>
     </row>
   </sheetData>
@@ -5372,7 +5362,7 @@
   <dimension ref="A1:K72"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A73" activeCellId="1" sqref="L110:L145 A73"/>
+      <selection pane="topLeft" activeCell="A73" activeCellId="1" sqref="C2:C145 A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6832,7 +6822,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49:E72">
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"LOC"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>